<commit_message>
Fixed app, added scaler
</commit_message>
<xml_diff>
--- a/data/sample_test.xlsx
+++ b/data/sample_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\spotifyproject\spotify-ml\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B98A8D-1D29-400A-AC8B-E024E63EB8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87ED5D1-88F1-4171-BD58-3A66DAE70981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04FFB06D-B898-41C1-B3FC-CC94B4F7A394}"/>
   </bookViews>
@@ -482,12 +482,13 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>